<commit_message>
tweaks and modifications to the report and functons used within
</commit_message>
<xml_diff>
--- a/inst/extdata/metabolon_v1.1_example.xlsx
+++ b/inst/extdata/metabolon_v1.1_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dh16508/Documents/moose/work/scripts/metaboprep/test/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pbrc-my.sharepoint.com/personal/david_hughes_pbrc_edu/Documents/research/projects/metaboprep_2.0/metaboprep_v2/metaboprep/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2EE66D-E92D-1148-9F83-C8C404FBFFAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{0A2EE66D-E92D-1148-9F83-C8C404FBFFAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27A1A2C5-D417-6F4A-A3F8-232D2F42ACC0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="10140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5780" yWindow="500" windowWidth="32620" windowHeight="18920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Explanation" sheetId="2" r:id="rId1"/>
@@ -1645,9 +1645,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1685,7 +1685,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1791,7 +1791,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1933,7 +1933,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1972,8 +1972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:DB107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36145,10 +36145,16 @@
   <dimension ref="A1:DA107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:105" x14ac:dyDescent="0.2">
       <c r="E1" s="2" t="s">

</xml_diff>